<commit_message>
DDL, DML E DQL Concluidos
</commit_message>
<xml_diff>
--- a/1.3-exercicio-pclinics/01_modelagem_fisico.xlsx
+++ b/1.3-exercicio-pclinics/01_modelagem_fisico.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F23634E-643B-4D89-9B06-F386FB40EFC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFD5CC7-CC07-4DE4-ABDC-4725B274825E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23790" yWindow="1680" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pclinics" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -320,13 +320,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -334,19 +349,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -356,40 +362,7 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -408,11 +381,50 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -698,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,26 +732,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="L1" s="20" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="L1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -754,34 +766,34 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -792,301 +804,301 @@
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="17">
+        <v>1</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="18">
         <v>43383</v>
       </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7">
-        <v>1</v>
-      </c>
-      <c r="M3" s="7" t="s">
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1</v>
+      </c>
+      <c r="L3" s="22">
+        <v>1</v>
+      </c>
+      <c r="M3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="23">
         <v>43852</v>
       </c>
-      <c r="O3" s="16">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="F4" s="17">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="18">
         <v>42873</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="17">
         <v>4</v>
       </c>
-      <c r="J4" s="11">
-        <v>1</v>
-      </c>
-      <c r="L4" s="7">
+      <c r="J4" s="17">
+        <v>1</v>
+      </c>
+      <c r="L4" s="22">
         <v>2</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="23">
         <v>43851</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="24">
         <v>2</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="24">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="F5" s="3">
+      <c r="B5" s="27"/>
+      <c r="F5" s="17">
         <v>3</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="18">
         <v>42537</v>
       </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="I5" s="17">
+        <v>1</v>
+      </c>
+      <c r="J5" s="17">
         <v>2</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="22">
         <v>3</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="23">
         <v>43852</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="24">
         <v>2</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
-        <v>1</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="17" t="s">
+      <c r="G8" s="30"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="F10" s="32">
-        <v>1</v>
-      </c>
-      <c r="G10" s="32" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="21">
+        <v>1</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="21">
         <v>432551</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="20">
         <v>2</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="14">
+      <c r="H11" s="13"/>
+      <c r="I11" s="21">
         <v>2</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="21">
         <v>653655</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="19">
+        <v>1</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="19">
         <v>2</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="19">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="19">
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="19">
         <v>2</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>